<commit_message>
modified some values and added virtual environment
</commit_message>
<xml_diff>
--- a/Workdays.xlsx
+++ b/Workdays.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janiz\OneDrive\Asztali gép\ProgrammingRelated\BK_v3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szlaveczfanni/Desktop/BurgerKingIncome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB62A2D-23D0-42A8-B6E4-54CFACF8942A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE37430C-2213-E140-9CBD-A4DB852B062A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{99A10659-EA22-4FA4-B535-98C45F486D9F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15580" activeTab="1" xr2:uid="{99A10659-EA22-4FA4-B535-98C45F486D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="60">
   <si>
     <t>November</t>
   </si>
@@ -206,14 +206,26 @@
     <t>17:05-18:49</t>
   </si>
   <si>
-    <t>17:45-22:30</t>
+    <t>18:00-1:30</t>
+  </si>
+  <si>
+    <t>19:00-0:00</t>
+  </si>
+  <si>
+    <t>11:00-18:30</t>
+  </si>
+  <si>
+    <t>10:00-16:00</t>
+  </si>
+  <si>
+    <t>10:00-18:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,7 +253,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Poppins"/>
-      <charset val="238"/>
     </font>
     <font>
       <b/>
@@ -253,8 +264,30 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFAADE"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +297,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAADE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,7 +370,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -328,6 +412,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFAADE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -642,13 +731,13 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="13.42578125" customWidth="1"/>
+    <col min="2" max="13" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -687,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
@@ -708,7 +797,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -727,7 +816,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -746,7 +835,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -765,7 +854,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
@@ -784,7 +873,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
@@ -803,7 +892,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
@@ -822,7 +911,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -841,7 +930,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
@@ -858,7 +947,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
@@ -875,7 +964,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
@@ -892,7 +981,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>24</v>
       </c>
@@ -909,7 +998,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
@@ -928,7 +1017,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
@@ -947,7 +1036,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -964,7 +1053,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -981,7 +1070,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>29</v>
       </c>
@@ -998,7 +1087,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>30</v>
       </c>
@@ -1015,7 +1104,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>31</v>
       </c>
@@ -1032,7 +1121,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -1049,7 +1138,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>33</v>
       </c>
@@ -1066,7 +1155,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>34</v>
       </c>
@@ -1083,7 +1172,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>35</v>
       </c>
@@ -1100,7 +1189,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>36</v>
       </c>
@@ -1117,7 +1206,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>37</v>
       </c>
@@ -1134,7 +1223,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>38</v>
       </c>
@@ -1151,7 +1240,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>39</v>
       </c>
@@ -1168,7 +1257,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>40</v>
       </c>
@@ -1185,7 +1274,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>41</v>
       </c>
@@ -1202,7 +1291,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>42</v>
       </c>
@@ -1219,7 +1308,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>43</v>
       </c>
@@ -1236,7 +1325,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1248,17 +1337,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEA11D6-5470-410F-863C-B064487B467F}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="117" workbookViewId="0">
+      <selection activeCell="H29" sqref="H28:H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="13.42578125" customWidth="1"/>
+    <col min="2" max="13" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -1297,17 +1386,817 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>49</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05640B-5C3A-4D6E-99A3-8B666B72D1C7}">
+  <dimension ref="A1:M33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1318,13 +2207,13 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="9"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1335,16 +2224,12 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1354,11 +2239,9 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -1375,13 +2258,11 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="B6" s="5"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1394,13 +2275,11 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1413,13 +2292,11 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1432,7 +2309,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -1449,7 +2326,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
@@ -1466,13 +2343,11 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1485,13 +2360,11 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1504,13 +2377,11 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1523,13 +2394,11 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1542,13 +2411,11 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1561,13 +2428,11 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1580,13 +2445,11 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1599,13 +2462,11 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1618,13 +2479,11 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1637,7 +2496,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>31</v>
       </c>
@@ -1654,7 +2513,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -1671,13 +2530,11 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1690,7 +2547,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>34</v>
       </c>
@@ -1707,7 +2564,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>35</v>
       </c>
@@ -1724,7 +2581,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>36</v>
       </c>
@@ -1741,7 +2598,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>37</v>
       </c>
@@ -1758,7 +2615,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>38</v>
       </c>
@@ -1775,7 +2632,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>39</v>
       </c>
@@ -1792,7 +2649,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>40</v>
       </c>
@@ -1809,7 +2666,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>41</v>
       </c>
@@ -1826,7 +2683,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>42</v>
       </c>
@@ -1843,7 +2700,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>43</v>
       </c>
@@ -1860,594 +2717,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05640B-5C3A-4D6E-99A3-8B666B72D1C7}">
-  <dimension ref="A1:M33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="13.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-    </row>
-    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2461,13 +2731,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="13.42578125" customWidth="1"/>
+    <col min="2" max="13" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -2506,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
@@ -2523,7 +2793,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -2540,7 +2810,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -2557,7 +2827,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2574,7 +2844,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
@@ -2591,7 +2861,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
@@ -2608,7 +2878,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
@@ -2625,7 +2895,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -2642,7 +2912,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
@@ -2659,7 +2929,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
@@ -2676,7 +2946,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
@@ -2693,7 +2963,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>24</v>
       </c>
@@ -2710,7 +2980,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
@@ -2727,7 +2997,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
@@ -2744,7 +3014,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -2761,7 +3031,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -2778,7 +3048,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>29</v>
       </c>
@@ -2795,7 +3065,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>30</v>
       </c>
@@ -2812,7 +3082,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>31</v>
       </c>
@@ -2829,7 +3099,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -2846,7 +3116,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>33</v>
       </c>
@@ -2863,7 +3133,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>34</v>
       </c>
@@ -2880,7 +3150,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>35</v>
       </c>
@@ -2897,7 +3167,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>36</v>
       </c>
@@ -2914,7 +3184,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>37</v>
       </c>
@@ -2931,7 +3201,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>38</v>
       </c>
@@ -2948,7 +3218,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>39</v>
       </c>
@@ -2965,7 +3235,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>40</v>
       </c>
@@ -2982,7 +3252,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>41</v>
       </c>
@@ -2999,7 +3269,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>42</v>
       </c>
@@ -3016,7 +3286,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>43</v>
       </c>
@@ -3033,7 +3303,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>